<commit_message>
Make some change to front end design..
</commit_message>
<xml_diff>
--- a/Moviesdb.xlsx
+++ b/Moviesdb.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Uid</t>
   </si>
@@ -92,7 +92,112 @@
     <t>tt5457772</t>
   </si>
   <si>
-    <t>Sarrainodu2017</t>
+    <t>Bhoothnath</t>
+  </si>
+  <si>
+    <t>06Bb4G7xB3k</t>
+  </si>
+  <si>
+    <t>Rascals</t>
+  </si>
+  <si>
+    <t>uA2x_yT61LI</t>
+  </si>
+  <si>
+    <t>Garam Masala</t>
+  </si>
+  <si>
+    <t>G9ZV4NZ5Ulw</t>
+  </si>
+  <si>
+    <t>gxBERAhEU7w</t>
+  </si>
+  <si>
+    <t>Tezz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungama </t>
+  </si>
+  <si>
+    <t>HVyXEbOWrp4</t>
+  </si>
+  <si>
+    <t>Hulchul</t>
+  </si>
+  <si>
+    <t>5QDKX5ExXqM</t>
+  </si>
+  <si>
+    <t>tt0991346</t>
+  </si>
+  <si>
+    <t>Comedy</t>
+  </si>
+  <si>
+    <t>Sarrainodu2017.jpg</t>
+  </si>
+  <si>
+    <t>Bhoothnath2008.jpg</t>
+  </si>
+  <si>
+    <t>tt1830786</t>
+  </si>
+  <si>
+    <t>tt0453671</t>
+  </si>
+  <si>
+    <t>tt1706317</t>
+  </si>
+  <si>
+    <t>Thriller</t>
+  </si>
+  <si>
+    <t>tt0371735</t>
+  </si>
+  <si>
+    <t>tt0437238</t>
+  </si>
+  <si>
+    <t>Rascals2011.jpg</t>
+  </si>
+  <si>
+    <t>Garam Masala2005.jpg</t>
+  </si>
+  <si>
+    <t>Tezz2012.jpg</t>
+  </si>
+  <si>
+    <t>Hungama2003.jpg</t>
+  </si>
+  <si>
+    <t>Hulchul2004.jpg</t>
+  </si>
+  <si>
+    <t>ACTOR</t>
+  </si>
+  <si>
+    <t>Amitabh Bachchan</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Salman Khan</t>
+  </si>
+  <si>
+    <t>Allu Arjun</t>
+  </si>
+  <si>
+    <t>Ajay Devgan</t>
+  </si>
+  <si>
+    <t>Akshay Kumar</t>
+  </si>
+  <si>
+    <t>Paresh Rawal</t>
+  </si>
+  <si>
+    <t>Akshaye Khanna</t>
   </si>
 </sst>
 </file>
@@ -416,25 +521,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I3" sqref="A3:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="3" max="3" width="16.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="12.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="10.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="21.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,48 +552,54 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2">
         <v>1080</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2008</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -496,23 +609,26 @@
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2">
         <v>1997</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1080</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -522,20 +638,197 @@
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2">
         <v>2017</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1">
         <v>1080</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2011</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2005</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2012</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2003</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1080</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2004</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>